<commit_message>
completed categorical variables exercise
</commit_message>
<xml_diff>
--- a/Statistics (Part 3)/2.3.Categorical-variables.Visualization-techniques-exercise.xlsx
+++ b/Statistics (Part 3)/2.3.Categorical-variables.Visualization-techniques-exercise.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB1D0FE-77A5-7D47-86AA-98B1A9D67392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0A7991-8359-714F-A26B-32307E5FF5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Frequency distribution table" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="16" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="17" r:id="rId1"/>
+    <sheet name="Frequency distribution table" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="13" r:id="rId3"/>
     <sheet name="Bar chart" sheetId="8" r:id="rId4"/>
     <sheet name="Pie chart" sheetId="7" r:id="rId5"/>
     <sheet name="Pareto diagram" sheetId="12" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
@@ -24,12 +24,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Background</t>
   </si>
@@ -120,12 +131,21 @@
   <si>
     <t>Frequency</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Relative Frequency</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +200,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -209,7 +235,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -227,13 +253,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -249,6 +283,2451 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Ice Cream Sold</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>New York</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Los Angeles</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>San Francisco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19923</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-556A-5041-94DC-32D9757210FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="697487168"/>
+        <c:axId val="697594176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="697487168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697594176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="697594176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697487168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Ice Cream Sold</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$4:$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>New York</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Los Angeles</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>San Francisco</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$4:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17129</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19923</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-30F5-304D-9DC8-B79A0DE00CE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="697487168"/>
+        <c:axId val="697594176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="697487168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697594176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="697594176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="697487168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>679450</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DA59A63-3CCE-F113-C76E-3522FB9D9111}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1652F2A3-38A9-D242-923D-DF17594256D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA7DDB1-758D-7EC8-BE6C-E511F30AF600}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -299,7 +2778,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{45E85198-C6B6-124F-B2EB-715B798C56C9}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="B15:C19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -353,60 +2832,28 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{011EF99A-A761-834C-B0B3-646844602A9B}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Frequency" fld="1" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{14EDD82E-E456-3844-83C9-C232D6BCDD19}" name="Table3" displayName="Table3" ref="D4:F8" totalsRowShown="0">
+  <autoFilter ref="D4:F8" xr:uid="{14EDD82E-E456-3844-83C9-C232D6BCDD19}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A5417E58-F489-D940-A2A9-3BD107CAA192}" name=" " dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9E02FB42-B312-F349-A896-6ABD4B9AF5FF}" name="Frequency"/>
+    <tableColumn id="3" xr3:uid="{A0E230A6-9BD4-3A44-AD45-82574B68BAA2}" name="Relative Frequency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3253B062-01EF-714F-9F25-21F462B35B82}" name="Table35" displayName="Table35" ref="B13:D17" totalsRowShown="0">
+  <autoFilter ref="B13:D17" xr:uid="{3253B062-01EF-714F-9F25-21F462B35B82}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6C7822FC-C9F0-244C-81F4-5CF24AB81A62}" name=" " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BA8451C8-4DC7-7A40-BF28-D46FEEB6CE46}" name="Frequency"/>
+    <tableColumn id="3" xr3:uid="{CBBCD3A7-EDC3-E340-B1ED-6B814717EC2E}" name="Relative Frequency"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,11 +3118,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97DBF2F-48DF-3F4D-8E34-13A6D6293D95}">
+  <dimension ref="A3:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>17129</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>12327</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>17129</v>
+      </c>
+      <c r="F5" s="13">
+        <f>E5/E8</f>
+        <v>0.34688835334858947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>19923</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>12327</v>
+      </c>
+      <c r="F6" s="13">
+        <f>E6/E8</f>
+        <v>0.24964053545029263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>49379</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>19923</v>
+      </c>
+      <c r="F7" s="13">
+        <f>E7/E8</f>
+        <v>0.40347111120111789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <f>SUBTOTAL(109,E5:E7)</f>
+        <v>49379</v>
+      </c>
+      <c r="F8" s="13">
+        <f>SUBTOTAL(109,F5:F7)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -741,112 +3304,15 @@
     <row r="14" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16">
-        <v>17129</v>
-      </c>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.15">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17">
-        <v>12327</v>
-      </c>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18">
-        <v>19923</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19">
-        <v>49379</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B164CB3-558A-0E41-BFE5-38D2005DCF0B}">
-  <dimension ref="A3:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4">
-        <v>17129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>12327</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>19923</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7">
-        <v>49379</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -854,8 +3320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F7A60E-A95B-6048-9274-B55E5296CDE4}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -898,6 +3364,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -905,7 +3372,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -982,14 +3451,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:E15"/>
+  <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1055,23 +3527,76 @@
       <c r="D12" s="5"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B13" s="2"/>
-      <c r="D13" s="5"/>
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B14" s="2"/>
-      <c r="D14" s="5"/>
+    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>17129</v>
+      </c>
+      <c r="D14" s="13">
+        <f>C14/C17</f>
+        <v>0.34688835334858947</v>
+      </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B15" s="2"/>
-      <c r="D15" s="7"/>
+    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>12327</v>
+      </c>
+      <c r="D15" s="13">
+        <f>C15/C17</f>
+        <v>0.24964053545029263</v>
+      </c>
       <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16">
+        <v>19923</v>
+      </c>
+      <c r="D16" s="13">
+        <f>C16/C17</f>
+        <v>0.40347111120111789</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <f>SUBTOTAL(109,C14:C16)</f>
+        <v>49379</v>
+      </c>
+      <c r="D17" s="13">
+        <f>SUBTOTAL(109,D14:D16)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1079,7 +3604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>